<commit_message>
Method reform and New testcases created
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -556,10 +556,10 @@
     <t>Testcc</t>
   </si>
   <si>
-    <t>Ranch</t>
-  </si>
-  <si>
-    <t>Rajaa</t>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Rani</t>
   </si>
 </sst>
 </file>
@@ -1299,7 +1299,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>

<commit_message>
Project Sync with Nitin's Changes and also updating the logic
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="183">
   <si>
     <t>Page/Section</t>
   </si>
@@ -502,9 +502,6 @@
     <t>Current Insurance Provider</t>
   </si>
   <si>
-    <t>MetLife</t>
-  </si>
-  <si>
     <t>Years with Current Insurer</t>
   </si>
   <si>
@@ -556,10 +553,25 @@
     <t>Testcc</t>
   </si>
   <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>Rani</t>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Vehicle</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>Auto Club Ent Insurance Group</t>
+  </si>
+  <si>
+    <t>Trufman</t>
+  </si>
+  <si>
+    <t>Raji</t>
   </si>
 </sst>
 </file>
@@ -980,7 +992,17 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1299,7 +1321,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1834,18 +1856,18 @@
     <mergeCell ref="A2:G2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:F24">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G24">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"FAILED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1864,10 +1886,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1917,582 +1939,602 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B7" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="8" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B8" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15" t="s">
+      <c r="C8" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15" t="s">
+      <c r="C9" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12" t="s">
+      <c r="C10" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="8" t="s">
+      <c r="C11" s="27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B12" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15" t="s">
+      <c r="C12" s="10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12" t="s">
+      <c r="C13" s="16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C14" s="13" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="8" t="s">
+    <row r="15" spans="1:3">
+      <c r="A15" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B15" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" s="16"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>97</v>
+      <c r="C15" s="10" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="14"/>
       <c r="B16" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>83</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="C16" s="16"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="14"/>
       <c r="B17" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C19" s="16" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="8" t="s">
+      <c r="C20" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B21" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C21" s="10" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="14"/>
-      <c r="B20" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="14"/>
       <c r="B22" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="14"/>
       <c r="B23" s="15" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="14"/>
       <c r="B24" s="15" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="14"/>
       <c r="B25" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="14"/>
+      <c r="B26" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="14"/>
+      <c r="B27" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C27" s="16" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="11"/>
-      <c r="B26" s="12" t="s">
+    <row r="28" spans="1:3">
+      <c r="A28" s="11"/>
+      <c r="B28" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C26" s="13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="8" t="s">
+      <c r="C28" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B29" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C29" s="10" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="14"/>
-      <c r="B28" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="14"/>
-      <c r="B29" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="14"/>
       <c r="B30" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="C30" s="16"/>
+        <v>75</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="14"/>
       <c r="B31" s="15" t="s">
-        <v>81</v>
+        <v>113</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="14"/>
       <c r="B32" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>117</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="C32" s="16"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="14"/>
       <c r="B33" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="14"/>
+      <c r="B34" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="14"/>
+      <c r="B35" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C33" s="16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="11"/>
-      <c r="B34" s="12" t="s">
+      <c r="C35" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="11"/>
+      <c r="B36" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="C34" s="13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="8" t="s">
+      <c r="C36" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B37" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C37" s="10" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="14"/>
-      <c r="B36" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="14"/>
-      <c r="B37" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="14"/>
       <c r="B38" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="14"/>
+      <c r="B39" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="14"/>
+      <c r="B40" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="C40" s="16" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="11"/>
-      <c r="B39" s="12" t="s">
+    <row r="41" spans="1:3">
+      <c r="A41" s="11"/>
+      <c r="B41" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C39" s="13"/>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="8" t="s">
+      <c r="C41" s="13"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B42" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C40" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="14"/>
-      <c r="B41" s="15" t="s">
+      <c r="C42" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="14"/>
+      <c r="B43" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="C43" s="16" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="11"/>
-      <c r="B42" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="11"/>
       <c r="B44" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C44" s="13"/>
+        <v>135</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="11"/>
+      <c r="B46" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46" s="13"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B47" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C45" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="14"/>
-      <c r="B46" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="C46" s="16" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="14"/>
-      <c r="B47" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>161</v>
+      <c r="C47" s="10" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="14"/>
       <c r="B48" s="15" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="14"/>
       <c r="B49" s="15" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="11"/>
-      <c r="B50" s="12" t="s">
+      <c r="A50" s="14"/>
+      <c r="B50" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="14"/>
+      <c r="B51" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="11"/>
+      <c r="B52" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C52" s="13" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="8" t="s">
+    <row r="53" spans="1:3">
+      <c r="A53" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B53" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C51" s="26" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="14"/>
-      <c r="B52" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="C52" s="16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="14"/>
-      <c r="B53" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="C53" s="16" t="s">
-        <v>15</v>
+      <c r="C53" s="26" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="14"/>
       <c r="B54" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="14"/>
+      <c r="B55" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="14"/>
+      <c r="B56" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="C54" s="16" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="11"/>
-      <c r="B55" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="C55" s="13" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="B56" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>145</v>
+      <c r="C56" s="16" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="11"/>
       <c r="B57" s="12" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="11"/>
+      <c r="B59" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="B58" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="14"/>
-      <c r="B59" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="C59" s="16" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="14"/>
-      <c r="B60" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="C60" s="16" t="s">
-        <v>169</v>
+      <c r="B60" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="14"/>
       <c r="B61" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="14"/>
+      <c r="B62" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="C62" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="C61" s="16" t="s">
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="14"/>
+      <c r="B63" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="28" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="28" t="s">
+      <c r="B64" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="C64" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="B62" s="29" t="s">
-        <v>171</v>
-      </c>
-      <c r="C62" s="30" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="8" t="s">
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="B63" s="9" t="s">
+      <c r="B65" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C65" s="10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="14"/>
+      <c r="B66" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C66" s="16" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="14"/>
-      <c r="B64" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="C64" s="16" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="14"/>
-      <c r="B65" s="15" t="s">
+    <row r="67" spans="1:3">
+      <c r="A67" s="14"/>
+      <c r="B67" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="C65" s="16" t="s">
+      <c r="C67" s="16" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="11"/>
-      <c r="B66" s="12" t="s">
+    <row r="68" spans="1:3">
+      <c r="A68" s="11"/>
+      <c r="B68" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="C66" s="27" t="s">
+      <c r="C68" s="27" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2500,12 +2542,15 @@
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B1:B59 B61:B1048576">
+  <conditionalFormatting sqref="B63:B1048576 B1:B61">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:B6">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" location="/v1-family"/>
-    <hyperlink ref="C51" r:id="rId2"/>
+    <hyperlink ref="C53" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Code change for json vehicle testdata  structure also new testcases tested
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8145" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8145" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BatchFile" sheetId="3" r:id="rId1"/>
     <sheet name="Quick Sanity" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BatchFile!$A$3:$F$13</definedName>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="232">
   <si>
     <t>Page/Section</t>
   </si>
@@ -572,6 +574,153 @@
   </si>
   <si>
     <t>Raji</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>PaperlessDiscount</t>
+  </si>
+  <si>
+    <t>E-SignatureDiscount</t>
+  </si>
+  <si>
+    <t>MaritalStatus</t>
+  </si>
+  <si>
+    <t>LicenseState</t>
+  </si>
+  <si>
+    <t>CustomEquipment</t>
+  </si>
+  <si>
+    <t>YearBought</t>
+  </si>
+  <si>
+    <t>MonthBought</t>
+  </si>
+  <si>
+    <t>HandsFree</t>
+  </si>
+  <si>
+    <t>CrashAvoidance</t>
+  </si>
+  <si>
+    <t>CardHolderFirstName</t>
+  </si>
+  <si>
+    <t>CardHolderLastName</t>
+  </si>
+  <si>
+    <t>s=</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Testk</t>
+  </si>
+  <si>
+    <t>Aboutyourfamily</t>
+  </si>
+  <si>
+    <t>LittleOnes</t>
+  </si>
+  <si>
+    <t>YoungAdults</t>
+  </si>
+  <si>
+    <t>StreetAddress</t>
+  </si>
+  <si>
+    <t>MoveinYear</t>
+  </si>
+  <si>
+    <t>MoveinMonth</t>
+  </si>
+  <si>
+    <t>TypeofResidence</t>
+  </si>
+  <si>
+    <t>Rentersinsuranceinterest</t>
+  </si>
+  <si>
+    <t>Financeorlease</t>
+  </si>
+  <si>
+    <t>KeptinZip</t>
+  </si>
+  <si>
+    <t>Ownedbyyou</t>
+  </si>
+  <si>
+    <t>Titledinnext30days</t>
+  </si>
+  <si>
+    <t>EstimatedValue</t>
+  </si>
+  <si>
+    <t>ValidLicense</t>
+  </si>
+  <si>
+    <t>Agefirstlicensed</t>
+  </si>
+  <si>
+    <t>IncidentHistory</t>
+  </si>
+  <si>
+    <t>IncidentDate</t>
+  </si>
+  <si>
+    <t>CurrentlyInsured</t>
+  </si>
+  <si>
+    <t>CurrentInsuranceProvider</t>
+  </si>
+  <si>
+    <t>YearswithCurrentInsurer</t>
+  </si>
+  <si>
+    <t>BILimit</t>
+  </si>
+  <si>
+    <t>Uninsuredinlast3years</t>
+  </si>
+  <si>
+    <t>PolicyStartDate</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>Licenseno</t>
+  </si>
+  <si>
+    <t>PaymentPlan</t>
+  </si>
+  <si>
+    <t>CardNo</t>
+  </si>
+  <si>
+    <t>ExpiryDate</t>
+  </si>
+  <si>
+    <t>PolicyholderDetails</t>
+  </si>
+  <si>
+    <t>InsuranceHistory</t>
+  </si>
+  <si>
+    <t>ConfirmDriver</t>
+  </si>
+  <si>
+    <t>ConfirmVehicle</t>
+  </si>
+  <si>
+    <t>V1</t>
   </si>
 </sst>
 </file>
@@ -666,7 +815,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -907,12 +1056,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="6" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -960,6 +1120,10 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -987,12 +1151,114 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1346,26 +1612,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="33"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="37"/>
     </row>
     <row r="2" spans="1:7" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="36"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="40"/>
     </row>
     <row r="3" spans="1:7" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
@@ -1856,18 +2122,18 @@
     <mergeCell ref="A2:G2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:F24">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G24">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>"FAILED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1888,8 +2154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1901,11 +2167,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="39"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="43"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="22" t="s">
@@ -2543,10 +2809,10 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="B63:B1048576 B1:B61">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B6">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" location="/v1-family"/>
@@ -2555,4 +2821,1854 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D80"/>
+  <sheetViews>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection sqref="A1:D80"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" style="17" customWidth="1"/>
+    <col min="2" max="3" width="32.140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="31"/>
+      <c r="B2" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="31"/>
+      <c r="B3" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="31"/>
+      <c r="B5" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="31"/>
+      <c r="B7" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="31"/>
+      <c r="B8" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="31"/>
+      <c r="B9" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="31"/>
+      <c r="B10" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="33"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="32"/>
+      <c r="B12" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="31"/>
+      <c r="B13" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="31"/>
+      <c r="B14" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="32"/>
+      <c r="B16" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="31"/>
+      <c r="B17" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D17" s="32"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="31"/>
+      <c r="B18" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="31"/>
+      <c r="B19" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="31"/>
+      <c r="B20" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="31"/>
+      <c r="B21" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="32"/>
+      <c r="B23" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="31"/>
+      <c r="B24" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="31"/>
+      <c r="B25" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="31"/>
+      <c r="B26" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="31"/>
+      <c r="B27" s="32" t="s">
+        <v>207</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="31"/>
+      <c r="B28" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="31"/>
+      <c r="B29" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="31"/>
+      <c r="B30" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="32"/>
+      <c r="B32" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="31"/>
+      <c r="B33" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="C33" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="31"/>
+      <c r="B34" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="C34" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="31"/>
+      <c r="B35" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="C35" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D35" s="32"/>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="31"/>
+      <c r="B36" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="C36" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="31"/>
+      <c r="B37" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="C37" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="31"/>
+      <c r="B38" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="C38" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D38" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="31"/>
+      <c r="B39" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="C39" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D39" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="32"/>
+      <c r="B41" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D41" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="31"/>
+      <c r="B42" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="C42" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D42" s="32" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="31"/>
+      <c r="B43" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D43" s="32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="31"/>
+      <c r="B44" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="C44" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D44" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="31"/>
+      <c r="B45" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C45" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D45" s="32"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="32"/>
+      <c r="B47" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="C47" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D47" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="31"/>
+      <c r="B48" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="C48" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D48" s="32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="31"/>
+      <c r="B49" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="C49" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D49" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="32"/>
+      <c r="B51" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D51" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="31"/>
+      <c r="B52" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="C52" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D52" s="32"/>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="B53" s="32"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="32"/>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="32"/>
+      <c r="B54" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="C54" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D54" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="31"/>
+      <c r="B55" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="C55" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D55" s="32" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="31"/>
+      <c r="B56" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="C56" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D56" s="32" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="31"/>
+      <c r="B57" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="C57" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D57" s="32" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="31"/>
+      <c r="B58" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="C58" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D58" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="31"/>
+      <c r="B59" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C59" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D59" s="32" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B60" s="32"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="32"/>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="32"/>
+      <c r="B61" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D61" s="34" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="31"/>
+      <c r="B62" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="C62" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D62" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="31"/>
+      <c r="B63" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="C63" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D63" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="31"/>
+      <c r="B64" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="C64" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D64" s="32" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="31"/>
+      <c r="B65" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="C65" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D65" s="32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="B66" s="32"/>
+      <c r="C66" s="32"/>
+      <c r="D66" s="32"/>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="32"/>
+      <c r="B67" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C67" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D67" s="32" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="31"/>
+      <c r="B68" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="C68" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D68" s="32" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="31" t="s">
+        <v>230</v>
+      </c>
+      <c r="B69" s="32"/>
+      <c r="C69" s="32"/>
+      <c r="D69" s="32"/>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="32"/>
+      <c r="B70" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="C70" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D70" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="31"/>
+      <c r="B71" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="C71" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D71" s="32" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="31"/>
+      <c r="B72" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="C72" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D72" s="32" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="31"/>
+      <c r="B73" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="C73" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D73" s="32" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="B74" s="32"/>
+      <c r="C74" s="32"/>
+      <c r="D74" s="32"/>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="32"/>
+      <c r="B75" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="C75" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D75" s="32" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="B76" s="32"/>
+      <c r="C76" s="32"/>
+      <c r="D76" s="32"/>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="32"/>
+      <c r="B77" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="C77" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D77" s="32" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="31"/>
+      <c r="B78" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="C78" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D78" s="32" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="31"/>
+      <c r="B79" s="32" t="s">
+        <v>225</v>
+      </c>
+      <c r="C79" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D79" s="32" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="31"/>
+      <c r="B80" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="C80" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D80" s="33" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B5:C5 B7:C71 C70:C73 B73:C1048576">
+    <cfRule type="duplicateValues" dxfId="9" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C3">
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D61" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E81"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="31"/>
+      <c r="B2" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="31"/>
+      <c r="B3" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="31"/>
+      <c r="B5" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="31"/>
+      <c r="B7" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="31"/>
+      <c r="B8" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="31"/>
+      <c r="B9" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="31"/>
+      <c r="B10" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="33"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="32"/>
+      <c r="B12" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="31"/>
+      <c r="B13" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="31"/>
+      <c r="B14" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="32"/>
+      <c r="B16" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="31"/>
+      <c r="B17" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D17" s="32"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="31"/>
+      <c r="B18" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="31"/>
+      <c r="B19" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="31"/>
+      <c r="B20" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="31"/>
+      <c r="B21" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="31"/>
+      <c r="B23" s="45" t="s">
+        <v>231</v>
+      </c>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="32"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="31"/>
+      <c r="C25" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="31"/>
+      <c r="C26" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="31"/>
+      <c r="C27" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="31"/>
+      <c r="C28" s="32" t="s">
+        <v>207</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="31"/>
+      <c r="C29" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="31"/>
+      <c r="C30" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="31"/>
+      <c r="C31" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="E31" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="31"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="32"/>
+      <c r="C33" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="E33" s="32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="31"/>
+      <c r="C34" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="E34" s="32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="31"/>
+      <c r="C35" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="D35" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="E35" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="31"/>
+      <c r="C36" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="E36" s="32"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="31"/>
+      <c r="C37" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="E37" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="31"/>
+      <c r="C38" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="D38" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="E38" s="32" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="31"/>
+      <c r="C39" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="D39" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="E39" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="31"/>
+      <c r="C40" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="D40" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="E40" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="32"/>
+      <c r="B42" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D42" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="31"/>
+      <c r="B43" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="C43" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D43" s="32" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="31"/>
+      <c r="B44" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D44" s="32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="31"/>
+      <c r="B45" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="C45" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D45" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="31"/>
+      <c r="B46" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D46" s="32"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="32"/>
+      <c r="B48" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="C48" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D48" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="31"/>
+      <c r="B49" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="C49" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D49" s="32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="31"/>
+      <c r="B50" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="C50" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D50" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="32"/>
+      <c r="B52" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="C52" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D52" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="31"/>
+      <c r="B53" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="C53" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D53" s="32"/>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="32"/>
+      <c r="B55" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="C55" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D55" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="31"/>
+      <c r="B56" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="C56" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D56" s="32" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="31"/>
+      <c r="B57" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="C57" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D57" s="32" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="31"/>
+      <c r="B58" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="C58" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D58" s="32" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="31"/>
+      <c r="B59" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="C59" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D59" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="31"/>
+      <c r="B60" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C60" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D60" s="32" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B61" s="32"/>
+      <c r="C61" s="32"/>
+      <c r="D61" s="32"/>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="32"/>
+      <c r="B62" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C62" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D62" s="34" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="31"/>
+      <c r="B63" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="C63" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D63" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="31"/>
+      <c r="B64" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="C64" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D64" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="31"/>
+      <c r="B65" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="C65" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D65" s="32" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="31"/>
+      <c r="B66" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="C66" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D66" s="32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="B67" s="32"/>
+      <c r="C67" s="32"/>
+      <c r="D67" s="32"/>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="32"/>
+      <c r="B68" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C68" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D68" s="32" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="31"/>
+      <c r="B69" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="C69" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D69" s="32" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="31" t="s">
+        <v>230</v>
+      </c>
+      <c r="B70" s="32"/>
+      <c r="C70" s="32"/>
+      <c r="D70" s="32"/>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="32"/>
+      <c r="B71" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="C71" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D71" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="31"/>
+      <c r="B72" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="C72" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D72" s="32" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="31"/>
+      <c r="B73" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="C73" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D73" s="32" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="31"/>
+      <c r="B74" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="C74" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D74" s="32" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="B75" s="32"/>
+      <c r="C75" s="32"/>
+      <c r="D75" s="32"/>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="32"/>
+      <c r="B76" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="C76" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D76" s="32" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="B77" s="32"/>
+      <c r="C77" s="32"/>
+      <c r="D77" s="32"/>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="32"/>
+      <c r="B78" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="C78" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D78" s="32" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="31"/>
+      <c r="B79" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="C79" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D79" s="32" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="31"/>
+      <c r="B80" s="32" t="s">
+        <v>225</v>
+      </c>
+      <c r="C80" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D80" s="32" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="31"/>
+      <c r="B81" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="C81" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D81" s="33" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C3">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:C5 B7:C23 B41:C72 C24:D40 C73:C81 B74:B81 B24">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D62" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>